<commit_message>
added few more Testcases in Testcases.xlsx
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94953523-34EF-47BB-9A36-47AA7AED92B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793B1A6-2F62-48F6-AD68-9AA4191AB41B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Trace and GigIt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Feature Name</t>
   </si>
@@ -103,6 +100,83 @@
     <t>1. Check whether the User/Owner has proper internet connection.
 2. Check whether all the fields are properly filled or not.
 3. User/Owner should be redirected to the respective homepage after SignUp</t>
+  </si>
+  <si>
+    <t>Animation Screen show URL</t>
+  </si>
+  <si>
+    <t>To show Url text entry box when long pressed on Logo of the animation screen</t>
+  </si>
+  <si>
+    <t>1. Long press on the logo at the start of the app
+2. Check whether URL text entry box is being displayed or not</t>
+  </si>
+  <si>
+    <t>1. URL text entry box has to be displayed.</t>
+  </si>
+  <si>
+    <t>Project Name: Trace and GigIt</t>
+  </si>
+  <si>
+    <t>Author: Leela Krishna Kosaraju</t>
+  </si>
+  <si>
+    <t>Connect to android device using charles proxi</t>
+  </si>
+  <si>
+    <t>An android device must be able to connect through charles proxi</t>
+  </si>
+  <si>
+    <t>1. Phone and Laptop are on same network.
+2. Phone is connected to laptop via charles proxi
+3. All API are getting recorded in charles proxi</t>
+  </si>
+  <si>
+    <t>1. Open charles proxi on the laptop.
+2. Enter the IP address of the laptop on the proxi network of the phone.
+3. Both the laptop and phone must be on same network
+4. Check whether phone is connected to charles proxi
+5. Check whether all the API that are accessed on mobile are recording on charles proxi or not</t>
+  </si>
+  <si>
+    <t>The application is successfully installed on an android device</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Successfully Executed</t>
+  </si>
+  <si>
+    <t>The application is successfully Uninstalled from an android device</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SignUp API </t>
+  </si>
+  <si>
+    <t>Input from Postman must be saved in Mysql</t>
+  </si>
+  <si>
+    <t>1. To keep user name and password to be save in mysql through api
+2. once the user is been registered same user details should not be accepted
+3. if password conditions are not met user signup shouldn’t happen
+4. to make shure that password is saved in encrypted format</t>
+  </si>
+  <si>
+    <t>1. Response status code must be 200
+2. Result type must be JSON</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -145,14 +219,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -172,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED73F4B5-901A-4F8A-AEBC-98F5FD6B36AD}" name="Table1" displayName="Table1" ref="A5:H23" totalsRowShown="0">
-  <autoFilter ref="A5:H23" xr:uid="{4791574D-0F10-4452-BA29-2C2481AB7338}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED73F4B5-901A-4F8A-AEBC-98F5FD6B36AD}" name="Table1" displayName="Table1" ref="A6:H24" totalsRowShown="0">
+  <autoFilter ref="A6:H24" xr:uid="{4791574D-0F10-4452-BA29-2C2481AB7338}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{2D0E096D-0D08-44D1-B007-74DB7B9EE04C}" name="Feature Name"/>
     <tableColumn id="2" xr3:uid="{A99706DF-BFCB-4900-B1C6-AFF3B8F53408}" name="Summary"/>
@@ -451,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H9"/>
+  <dimension ref="A3:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
@@ -471,91 +553,186 @@
     <col min="10" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small update to test cases
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793B1A6-2F62-48F6-AD68-9AA4191AB41B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,11 +51,6 @@
     <t>Verify that the application is installed successfully.</t>
   </si>
   <si>
-    <t>1. Search for the application from google play
-2. Click on install button
-3. Open the application</t>
-  </si>
-  <si>
     <t>The application should be installed successfully</t>
   </si>
   <si>
@@ -178,11 +172,15 @@
   <si>
     <t>Failed</t>
   </si>
+  <si>
+    <t>1. Installing through APK file 
+2. Open the application</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,17 +252,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED73F4B5-901A-4F8A-AEBC-98F5FD6B36AD}" name="Table1" displayName="Table1" ref="A6:H24" totalsRowShown="0">
-  <autoFilter ref="A6:H24" xr:uid="{4791574D-0F10-4452-BA29-2C2481AB7338}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A6:H24" totalsRowShown="0">
+  <autoFilter ref="A6:H24"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2D0E096D-0D08-44D1-B007-74DB7B9EE04C}" name="Feature Name"/>
-    <tableColumn id="2" xr3:uid="{A99706DF-BFCB-4900-B1C6-AFF3B8F53408}" name="Summary"/>
-    <tableColumn id="3" xr3:uid="{3894421F-A889-483F-9A05-5EDDE991ABF1}" name="Execution Steps"/>
-    <tableColumn id="4" xr3:uid="{39009BDE-0A91-469F-9BC1-51B9E97DF2D5}" name="Expected Results"/>
-    <tableColumn id="5" xr3:uid="{02996EBF-CAD7-44C4-BEDF-28C82DD3FFD3}" name="Actual Result"/>
-    <tableColumn id="6" xr3:uid="{E325B7E2-10D8-4CA3-9341-DA0ECD18B1DC}" name="Priority"/>
-    <tableColumn id="7" xr3:uid="{91CFCB9C-A531-4898-A203-9C1C51A333BF}" name="Execution Status"/>
-    <tableColumn id="8" xr3:uid="{FA13DAEF-7875-4752-915F-B2285E2F60B2}" name="Comments"/>
+    <tableColumn id="1" name="Feature Name"/>
+    <tableColumn id="2" name="Summary"/>
+    <tableColumn id="3" name="Execution Steps"/>
+    <tableColumn id="4" name="Expected Results"/>
+    <tableColumn id="5" name="Actual Result"/>
+    <tableColumn id="6" name="Priority"/>
+    <tableColumn id="7" name="Execution Status"/>
+    <tableColumn id="8" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,12 +553,12 @@
   <sheetData>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -597,142 +595,142 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testcases updated for both front end and back end in Testcases.xlsx
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C7ED69-B16D-4620-A8E3-75892A0A54F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Feature Name</t>
   </si>
@@ -115,24 +117,6 @@
     <t>Author: Leela Krishna Kosaraju</t>
   </si>
   <si>
-    <t>Connect to android device using charles proxi</t>
-  </si>
-  <si>
-    <t>An android device must be able to connect through charles proxi</t>
-  </si>
-  <si>
-    <t>1. Phone and Laptop are on same network.
-2. Phone is connected to laptop via charles proxi
-3. All API are getting recorded in charles proxi</t>
-  </si>
-  <si>
-    <t>1. Open charles proxi on the laptop.
-2. Enter the IP address of the laptop on the proxi network of the phone.
-3. Both the laptop and phone must be on same network
-4. Check whether phone is connected to charles proxi
-5. Check whether all the API that are accessed on mobile are recording on charles proxi or not</t>
-  </si>
-  <si>
     <t>The application is successfully installed on an android device</t>
   </si>
   <si>
@@ -160,28 +144,55 @@
     <t>Input from Postman must be saved in Mysql</t>
   </si>
   <si>
-    <t>1. To keep user name and password to be save in mysql through api
+    <t>1. Response status code must be 200
+2. Result type must be JSON</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>1. Installing through APK file 
+2. Open the application</t>
+  </si>
+  <si>
+    <t>Status Result: 500 (Internal Server error)</t>
+  </si>
+  <si>
+    <t>Backend Testing</t>
+  </si>
+  <si>
+    <t>Frontend Testing</t>
+  </si>
+  <si>
+    <t>Register Device API</t>
+  </si>
+  <si>
+    <t>When a user install application in a device, on app launch this API should be called so that a session will be created for the device</t>
+  </si>
+  <si>
+    <t>1. To keep user name and password to be save in mysql through API
 2. once the user is been registered same user details should not be accepted
 3. if password conditions are not met user signup shouldn’t happen
-4. to make shure that password is saved in encrypted format</t>
-  </si>
-  <si>
-    <t>1. Response status code must be 200
-2. Result type must be JSON</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>1. Installing through APK file 
-2. Open the application</t>
+4. to make sure that password is saved in encrypted format</t>
+  </si>
+  <si>
+    <t>1. On applaunch register API must be called.
+2. If returning user on the same device, user will already be added to session else new session will be created.
+3. Check whether data is available or inserted in the session table and device table.</t>
+  </si>
+  <si>
+    <t>1. API should produce 200 response code.
+2. In response, client key must be present.
+3. There should valid records in tha database.
+4. If returning user, client key must be updated and new key must not be generated.
+5. when inserting in a session table, device must be attached to the session.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +202,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -217,28 +242,154 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -252,17 +403,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A6:H24" totalsRowShown="0">
-  <autoFilter ref="A6:H24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:H18" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A6:H18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Feature Name"/>
-    <tableColumn id="2" name="Summary"/>
-    <tableColumn id="3" name="Execution Steps"/>
-    <tableColumn id="4" name="Expected Results"/>
-    <tableColumn id="5" name="Actual Result"/>
-    <tableColumn id="6" name="Priority"/>
-    <tableColumn id="7" name="Execution Status"/>
-    <tableColumn id="8" name="Comments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Summary" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Execution Steps" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Expected Results" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Priority" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Execution Status" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Comments" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{01EABFC7-5928-4E82-8F8E-935B8E6DA2B5}" name="Table2" displayName="Table2" ref="A6:H28" totalsRowShown="0">
+  <autoFilter ref="A6:H28" xr:uid="{72BC6623-9889-4626-A85B-6D865FC00DC6}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1397C4C4-AEA2-4864-939A-1B812ECB6ABF}" name="Feature Name"/>
+    <tableColumn id="2" xr3:uid="{86399DDB-7304-4241-841A-CDCAFFFDB7A2}" name="Summary"/>
+    <tableColumn id="3" xr3:uid="{C697A405-BEFE-42D6-94F8-6B0A3F4E0B29}" name="Execution Steps"/>
+    <tableColumn id="4" xr3:uid="{B7DACE71-CD48-4155-ADB7-0784E7189FFC}" name="Expected Results"/>
+    <tableColumn id="5" xr3:uid="{52746B4B-F6CF-4A97-A9D8-59410302A1E5}" name="Actual Result"/>
+    <tableColumn id="6" xr3:uid="{AED13CB9-E0D6-4F06-8E9E-91B914A0C23E}" name="Priority"/>
+    <tableColumn id="7" xr3:uid="{4CA8DA74-0F06-4B3A-8A19-88E4D2DDC517}" name="Execution Status"/>
+    <tableColumn id="8" xr3:uid="{1022E392-8C5B-477B-9C58-3EAE25ACF0E6}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,11 +698,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +710,7 @@
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
@@ -552,13 +720,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,151 +760,149 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -740,4 +911,191 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A32A1C-5C45-4EBA-BB6F-C2AAA971ED99}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tested a Testcases.xlsx and noted the failures
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C7ED69-B16D-4620-A8E3-75892A0A54F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CEF44A-305D-4AA6-80FD-83770E64C935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Feature Name</t>
   </si>
@@ -106,9 +106,6 @@
   <si>
     <t>1. Long press on the logo at the start of the app
 2. Check whether URL text entry box is being displayed or not</t>
-  </si>
-  <si>
-    <t>1. URL text entry box has to be displayed.</t>
   </si>
   <si>
     <t>Project Name: Trace and GigIt</t>
@@ -186,6 +183,14 @@
 3. There should valid records in tha database.
 4. If returning user, client key must be updated and new key must not be generated.
 5. when inserting in a session table, device must be attached to the session.</t>
+  </si>
+  <si>
+    <t>1. URL text entry box has to be displayed.
+2. After entering the IP address, it should redirect to the login screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. After entering IP address, it is not redirecting to the login screen
+</t>
   </si>
 </sst>
 </file>
@@ -403,17 +408,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:H18" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:H18" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A6:H18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Summary" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Execution Steps" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Expected Results" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Actual Result" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Priority" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Execution Status" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Comments" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature Name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Summary" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Execution Steps" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Expected Results" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Actual Result" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Priority" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Execution Status" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="99" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="99" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -721,17 +726,17 @@
   <sheetData>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,44 +767,44 @@
     </row>
     <row r="7" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -917,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A32A1C-5C45-4EBA-BB6F-C2AAA971ED99}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,17 +940,17 @@
   <sheetData>
     <row r="1" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -982,22 +987,22 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -1014,16 +1019,16 @@
         <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1041,10 +1046,10 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -1063,10 +1068,10 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -1081,14 +1086,16 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H11" s="5"/>
     </row>

</xml_diff>

<commit_message>
updated Testcases.xlsx with signUP api and register device api successful and new testcase
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -3,25 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2D553C-63BF-4B1E-BB05-57B2A288B37D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7629A6-F428-49C8-9B72-BD84255EBDDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Feature Name</t>
   </si>
@@ -190,10 +196,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Test case is failing if we change fields like profile,make and model
-</t>
-  </si>
-  <si>
     <t>Network Connection</t>
   </si>
   <si>
@@ -212,14 +214,44 @@
     <t>1. We connected to the server and got timed out</t>
   </si>
   <si>
-    <t>1. We couldn't enter another device details.
-2. Should check if the values are hard-coded or not</t>
-  </si>
-  <si>
-    <t>1. Session ID missing.</t>
-  </si>
-  <si>
-    <t>It happened because register device API has failed.</t>
+    <t xml:space="preserve">1. Session ID has been created.
+2.User has been created but first name and last name fields are not mandatory. </t>
+  </si>
+  <si>
+    <t>partially successful</t>
+  </si>
+  <si>
+    <t>Some of the fields such firstname, lastname, gender are storing default values. They should be made mandatory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Device has been registered successfully.
+2. Client key has been generated.
+</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+  <si>
+    <t>Sign In API</t>
+  </si>
+  <si>
+    <t>Input Username and password from Postman</t>
+  </si>
+  <si>
+    <t>1. Enter Username and Password
+2. Click on Login
+3. Response code must be 200 which means successful</t>
+  </si>
+  <si>
+    <t>1. Correct Username and Password has been created
+2. Response code is successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is able to login just with session id
+</t>
+  </si>
+  <si>
+    <t>Username and password fields for login are not mandatory whoich should be fixed</t>
   </si>
 </sst>
 </file>
@@ -276,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -292,6 +324,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,17 +846,15 @@
         <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>54</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -834,33 +870,33 @@
         <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>28</v>
@@ -870,15 +906,31 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -973,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A32A1C-5C45-4EBA-BB6F-C2AAA971ED99}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added some more testcases to Testcases.xlsx
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7629A6-F428-49C8-9B72-BD84255EBDDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88779558-9D85-4821-8AFF-C56E25592C93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Feature Name</t>
   </si>
@@ -149,9 +149,6 @@
   <si>
     <t>1. Response status code must be 200
 2. Result type must be JSON</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
   <si>
     <t>1. Installing through APK file 
@@ -192,10 +189,6 @@
 2. After entering the IP address, it should redirect to the login screen.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. After entering IP address, it is not redirecting to the login screen
-</t>
-  </si>
-  <si>
     <t>Network Connection</t>
   </si>
   <si>
@@ -252,6 +245,25 @@
   </si>
   <si>
     <t>Username and password fields for login are not mandatory whoich should be fixed</t>
+  </si>
+  <si>
+    <t>Location screen</t>
+  </si>
+  <si>
+    <t>TO open location access when clicked on location button</t>
+  </si>
+  <si>
+    <t>1. click on location symbol on the home page of the screen
+2. click on settings on the pop up screen.
+3. give location access to the app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Location of the user must be accessed when clicked on location symbol.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login screen has been shown after entering IP address
+</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -329,6 +341,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="99" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="99" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +827,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,25 +858,25 @@
     </row>
     <row r="7" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -864,39 +888,39 @@
         <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>28</v>
@@ -908,28 +932,28 @@
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1023,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A32A1C-5C45-4EBA-BB6F-C2AAA971ED99}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1077,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,7 +1114,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1189,23 +1213,46 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated all the testcases in the Testcases.xlsx
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88779558-9D85-4821-8AFF-C56E25592C93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C99A0A9-24A7-4573-A3F5-2EAB6C334B51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>Feature Name</t>
   </si>
@@ -76,11 +76,6 @@
   </si>
   <si>
     <t>User/ Owner should be able to login in the application</t>
-  </si>
-  <si>
-    <t>1. Check whether the User/Owner has proper internet connection
-2. Check whether the username and password are correct.
-3. Check whether the User/Owner is able to see the home page of the application</t>
   </si>
   <si>
     <t>1. User/Owner has proper internet connection
@@ -133,9 +128,6 @@
   </si>
   <si>
     <t>The application is successfully Uninstalled from an android device</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
   <si>
     <t>Medium</t>
@@ -207,16 +199,6 @@
     <t>1. We connected to the server and got timed out</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Session ID has been created.
-2.User has been created but first name and last name fields are not mandatory. </t>
-  </si>
-  <si>
-    <t>partially successful</t>
-  </si>
-  <si>
-    <t>Some of the fields such firstname, lastname, gender are storing default values. They should be made mandatory.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Device has been registered successfully.
 2. Client key has been generated.
 </t>
@@ -240,13 +222,6 @@
 2. Response code is successful</t>
   </si>
   <si>
-    <t xml:space="preserve">1. User is able to login just with session id
-</t>
-  </si>
-  <si>
-    <t>Username and password fields for login are not mandatory whoich should be fixed</t>
-  </si>
-  <si>
     <t>Location screen</t>
   </si>
   <si>
@@ -264,6 +239,33 @@
   <si>
     <t xml:space="preserve">1. Login screen has been shown after entering IP address
 </t>
+  </si>
+  <si>
+    <t>1. Check whether the User/Owner has proper internet connection
+2. Check whether the username and password are correct.
+3. Password must be between 6-32 letters.
+4. Check whether the User/Owner is able to see the home page of the application</t>
+  </si>
+  <si>
+    <t>1. User is able to signup.</t>
+  </si>
+  <si>
+    <t>1. User is able to Login.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Location of the user has been accessed
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Session ID has been created.
+2.User has been created </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is able to login 
+</t>
+  </si>
+  <si>
+    <t>Susccessful</t>
   </si>
 </sst>
 </file>
@@ -797,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="99" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,17 +819,17 @@
   <sheetData>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,103 +860,99 @@
     </row>
     <row r="7" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1049,15 +1047,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A32A1C-5C45-4EBA-BB6F-C2AAA971ED99}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -1067,17 +1065,17 @@
   <sheetData>
     <row r="1" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,22 +1112,22 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,19 +1144,19 @@
         <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1166,86 +1164,100 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="F12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>32</v>
+      <c r="H12" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>